<commit_message>
Update to add latest changes
</commit_message>
<xml_diff>
--- a/Clustered_Outcome.xlsx
+++ b/Clustered_Outcome.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Koushik Karmakar\Desktop\projects\Data-Science-Capstone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{5C469C25-EE16-4394-930C-A736A4569285}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE882F77-AFD3-4436-9B01-AAD0A9B7ECCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Clustered_outcome" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15212" uniqueCount="834">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5872" uniqueCount="834">
   <si>
     <t>Borough</t>
   </si>
@@ -2530,7 +2530,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -3556,12 +3556,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P489"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:P1"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28032,7 +28032,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:P1"/>
+  <autoFilter ref="A1:P1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>